<commit_message>
updated maps and tables
</commit_message>
<xml_diff>
--- a/Data/Post1790/GA/T694_GA_Loan_Office_CD.xlsx
+++ b/Data/Post1790/GA/T694_GA_Loan_Office_CD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghall\Documents\Fiscal_History\Loan_Office_Project\Georgia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisliao/Google Drive/Non-Academic Work/Research/Sargent/SPEOC-pt-1/Data/Post1790/GA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC37EAC9-2F07-49B2-B8E9-C509D3A7C19E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6919C24-944E-EE4B-A53C-16A1532C7180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28230" yWindow="570" windowWidth="27225" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -851,6 +851,27 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -871,27 +892,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1249,24 +1249,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:U1048576"/>
+      <selection pane="bottomLeft" activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="7.25" style="11" customWidth="1"/>
-    <col min="3" max="13" width="7.25" style="7" customWidth="1"/>
-    <col min="14" max="14" width="7.58203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="11" customWidth="1"/>
+    <col min="3" max="13" width="7.1640625" style="7" customWidth="1"/>
+    <col min="14" max="14" width="7.5" style="7" customWidth="1"/>
     <col min="15" max="15" width="13.5" style="20" customWidth="1"/>
-    <col min="16" max="16" width="13.58203125" style="7" customWidth="1"/>
-    <col min="17" max="17" width="15.08203125" style="19" customWidth="1"/>
+    <col min="16" max="16" width="13.5" style="7" customWidth="1"/>
+    <col min="17" max="17" width="15" style="19" customWidth="1"/>
     <col min="18" max="18" width="14.83203125" style="6" customWidth="1"/>
-    <col min="19" max="19" width="18.25" style="20" customWidth="1"/>
-    <col min="20" max="20" width="8.25" style="20" customWidth="1"/>
+    <col min="19" max="19" width="18.1640625" style="20" customWidth="1"/>
+    <col min="20" max="20" width="8.1640625" style="20" customWidth="1"/>
     <col min="21" max="21" width="19.5" style="7" customWidth="1"/>
     <col min="22" max="22" width="10.33203125" style="7" customWidth="1"/>
     <col min="23" max="23" width="7.83203125" style="7" customWidth="1"/>
@@ -1282,7 +1282,7 @@
     <col min="33" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1320,7 +1320,7 @@
       <c r="AE1" s="42"/>
       <c r="AF1" s="49"/>
     </row>
-    <row r="2" spans="1:33" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1357,7 +1357,7 @@
       <c r="AE2" s="42"/>
       <c r="AF2" s="49"/>
     </row>
-    <row r="3" spans="1:33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="AE3" s="42"/>
       <c r="AF3" s="49"/>
     </row>
-    <row r="4" spans="1:33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1432,7 +1432,7 @@
       <c r="AE4" s="42"/>
       <c r="AF4" s="49"/>
     </row>
-    <row r="5" spans="1:33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1470,7 +1470,7 @@
       <c r="AE5" s="42"/>
       <c r="AF5" s="49"/>
     </row>
-    <row r="6" spans="1:33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1506,7 +1506,7 @@
       <c r="AE6" s="42"/>
       <c r="AF6" s="49"/>
     </row>
-    <row r="7" spans="1:33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1543,7 +1543,7 @@
       <c r="AE7" s="42"/>
       <c r="AF7" s="49"/>
     </row>
-    <row r="8" spans="1:33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1580,7 +1580,7 @@
       <c r="AE8" s="42"/>
       <c r="AF8" s="49"/>
     </row>
-    <row r="9" spans="1:33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1608,100 +1608,100 @@
       <c r="W9" s="2"/>
       <c r="X9" s="24"/>
       <c r="Y9" s="2"/>
-      <c r="Z9" s="62" t="s">
+      <c r="Z9" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="AA9" s="62"/>
-      <c r="AB9" s="65" t="s">
+      <c r="AA9" s="55"/>
+      <c r="AB9" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AC9" s="65"/>
+      <c r="AC9" s="58"/>
       <c r="AD9" s="35" t="s">
         <v>33</v>
       </c>
       <c r="AE9" s="47"/>
       <c r="AF9" s="49"/>
     </row>
-    <row r="10" spans="1:33" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="52" t="s">
+    <row r="10" spans="1:33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="58">
-        <v>1</v>
-      </c>
-      <c r="G10" s="58">
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="65">
+        <v>1</v>
+      </c>
+      <c r="G10" s="65">
         <v>2</v>
       </c>
-      <c r="H10" s="58">
+      <c r="H10" s="65">
         <v>3</v>
       </c>
-      <c r="I10" s="58">
+      <c r="I10" s="65">
         <v>4</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="57" t="s">
+      <c r="N10" s="53"/>
+      <c r="O10" s="53"/>
+      <c r="P10" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="Q10" s="57" t="s">
+      <c r="Q10" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="R10" s="57" t="s">
+      <c r="R10" s="64" t="s">
         <v>157</v>
       </c>
-      <c r="S10" s="63" t="s">
+      <c r="S10" s="56" t="s">
         <v>20</v>
       </c>
       <c r="T10" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="U10" s="64" t="s">
+      <c r="U10" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="V10" s="56" t="s">
+      <c r="V10" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="W10" s="56"/>
-      <c r="X10" s="54" t="s">
+      <c r="W10" s="63"/>
+      <c r="X10" s="61" t="s">
         <v>151</v>
       </c>
       <c r="Y10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Z10" s="62" t="s">
+      <c r="Z10" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="AA10" s="62"/>
-      <c r="AB10" s="65" t="s">
+      <c r="AA10" s="55"/>
+      <c r="AB10" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="AC10" s="65"/>
+      <c r="AC10" s="58"/>
       <c r="AD10" s="35" t="s">
         <v>25</v>
       </c>
       <c r="AE10" s="48"/>
-      <c r="AF10" s="61" t="s">
+      <c r="AF10" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="AG10" s="59" t="s">
+      <c r="AG10" s="52" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:33" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
-      <c r="B11" s="53"/>
+    <row r="11" spans="1:33" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="59"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="12" t="s">
         <v>0</v>
       </c>
@@ -1711,10 +1711,10 @@
       <c r="E11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
       <c r="J11" s="14" t="s">
         <v>52</v>
       </c>
@@ -1733,19 +1733,19 @@
       <c r="O11" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="57"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="63"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="64"/>
+      <c r="S11" s="56"/>
       <c r="T11" s="51"/>
-      <c r="U11" s="64"/>
+      <c r="U11" s="57"/>
       <c r="V11" s="10" t="s">
         <v>17</v>
       </c>
       <c r="W11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="X11" s="54"/>
+      <c r="X11" s="61"/>
       <c r="Y11" s="2" t="s">
         <v>30</v>
       </c>
@@ -1767,10 +1767,10 @@
       <c r="AE11" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="AF11" s="61"/>
-      <c r="AG11" s="59"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="AF11" s="54"/>
+      <c r="AG11" s="52"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>1</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>142.66999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>1</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>1905.7</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>1</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>228.9</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>2</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>4189.5599999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>2</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>2559.2299999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>5</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>648.30999999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>6</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>152.31</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>7</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>123.13</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>7</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>295.83999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>8</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>118.32</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>8</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>341.26659999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>9</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>2178.1566000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>9</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>648.3066</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>9</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>133.48660000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>11</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>339.4366</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>11</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>834.09659999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>12</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>859.17000000000007</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>12</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>556.17660000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>13</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>270.55</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
         <v>13</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>17892.756600000001</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
         <v>14</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>15</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>7496.73</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <v>15</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>3381.5365999999995</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
         <v>16</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>2367.3500000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
         <v>17</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>5914.5300000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <v>18</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>9607.5266000000011</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>18</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>7.9565999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" s="11">
         <v>18</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>741.56999999999994</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
         <v>19</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>1746.1266000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
         <v>19</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>568.33000000000004</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
         <v>19</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>193.48659999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
         <v>20</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>285.83999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
         <v>20</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>354.1</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
         <v>21</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>2767.8</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
         <v>21</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>295.14999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
         <v>22</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>3758.2799999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
         <v>22</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>474.01</v>
       </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A49" s="11">
         <v>23</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>2319.3362999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A50" s="11">
         <v>23</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>961.95659999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A51" s="11">
         <v>23</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>911.52659999999992</v>
       </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A52" s="11">
         <v>24</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>8.8666</v>
       </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A53" s="11">
         <v>24</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>13.026599999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A54" s="11">
         <v>24</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>442.51000000000005</v>
       </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A55" s="11">
         <v>24</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>505.35</v>
       </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A56" s="11">
         <v>25</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>283.15660000000003</v>
       </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A57" s="11">
         <v>25</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>176.25659999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A58" s="11">
         <v>25</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>345.82</v>
       </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A59" s="11">
         <v>25</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>338.40999999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A60" s="11">
         <v>26</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>177.82659999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A61" s="11">
         <v>26</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>2515.8065999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A62" s="11">
         <v>26</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>3561.8166000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A63" s="11">
         <v>27</v>
       </c>
@@ -5941,7 +5941,7 @@
         <v>9035.25</v>
       </c>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A64" s="11">
         <v>31</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>1677.04</v>
       </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A65" s="11">
         <v>32</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>68.429999999999993</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A66" s="11">
         <v>35</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>1686.6799999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A67" s="11">
         <v>43</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>39.18</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A68" s="11">
         <v>47</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>883.77</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A69" s="11">
         <v>48</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>826.77</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A70" s="11">
         <v>51</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>160.07999999999998</v>
       </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A71" s="11">
         <v>51</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>370.95000000000005</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A72" s="11">
         <v>53</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>478.64</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A73" s="11">
         <v>54</v>
       </c>
@@ -6757,7 +6757,7 @@
         <v>478.64</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A74" s="11">
         <v>55</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>89.53</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A75" s="11">
         <v>68</v>
       </c>
@@ -6919,7 +6919,7 @@
         <v>27.29</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A76" s="11">
         <v>76</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>23985.599999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
       <c r="AA78" s="45">
         <f>SUM(AA12:AA76)</f>
         <v>58168.251900000003</v>
@@ -7013,15 +7013,6 @@
     <sortCondition ref="A12:A76"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="AG10:AG11"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="AF10:AF11"/>
-    <mergeCell ref="Z9:AA9"/>
-    <mergeCell ref="S10:S11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="Z10:AA10"/>
-    <mergeCell ref="AB10:AC10"/>
-    <mergeCell ref="AB9:AC9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="X10:X11"/>
@@ -7034,6 +7025,15 @@
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I10:I11"/>
+    <mergeCell ref="AG10:AG11"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="AF10:AF11"/>
+    <mergeCell ref="Z9:AA9"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="Z10:AA10"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="AB9:AC9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>